<commit_message>
Ajustes de letra en archivo de excel
</commit_message>
<xml_diff>
--- a/images/evolucion.xlsx
+++ b/images/evolucion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e754af3616dfda6/Documentos/Developments/raios/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9F688A62-301A-461F-959B-8E49D14D3291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F8B632D-593A-417C-9C48-53657EF43D6E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{9F688A62-301A-461F-959B-8E49D14D3291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF667E19-60B5-4CE7-8EA1-B8960DDFF324}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C221C332-E014-436B-80AF-3F7DC92C09EC}"/>
   </bookViews>
@@ -623,7 +623,7 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>145831</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2340064" cy="441659"/>
+    <xdr:ext cx="3196068" cy="435247"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="CuadroTexto 13">
@@ -638,7 +638,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3883900" y="5670331"/>
-          <a:ext cx="2340064" cy="441659"/>
+          <a:ext cx="3196068" cy="435247"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -667,13 +667,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Manejo</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t> de inventario manual en excel</a:t>
           </a:r>
@@ -681,12 +683,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Tiempo Ejecución: 3 días</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -941,7 +945,7 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>44011</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3146952" cy="616323"/>
+    <xdr:ext cx="4109715" cy="606705"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="27" name="CuadroTexto 26">
@@ -956,7 +960,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6005347" y="4425511"/>
-          <a:ext cx="3146952" cy="616323"/>
+          <a:ext cx="4109715" cy="606705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -985,13 +989,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Semi-automatización</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t> de Cruces de inventario con</a:t>
           </a:r>
@@ -999,7 +1005,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Google Apps Scripts y Google Sheets</a:t>
           </a:r>
@@ -1007,12 +1014,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Tiempo Ejecución: 12.75 Horas</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -1314,7 +1323,7 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>158311</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3814057" cy="616323"/>
+    <xdr:ext cx="5099409" cy="606705"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="47" name="CuadroTexto 46">
@@ -1329,7 +1338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7957972" y="3396811"/>
-          <a:ext cx="3814057" cy="616323"/>
+          <a:ext cx="5099409" cy="606705"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1358,13 +1367,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Desarrollo</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t> de RAIOS</a:t>
           </a:r>
@@ -1372,7 +1383,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Plataforma Web, Cruces automáticos, Generación de informes</a:t>
           </a:r>
@@ -1380,12 +1392,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Tiempo Ejecución: 0,5 Horas</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -1506,7 +1520,7 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>120211</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2513124" cy="441659"/>
+    <xdr:ext cx="3209918" cy="435247"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="53" name="CuadroTexto 52">
@@ -1521,7 +1535,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9053347" y="2596711"/>
-          <a:ext cx="2513124" cy="441659"/>
+          <a:ext cx="3209918" cy="435247"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1550,7 +1564,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Migración de RAIOS  la Nube de Azure</a:t>
           </a:r>
@@ -1558,12 +1573,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Seguridad, Escalabilidad, Integridad</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2096,11 +2113,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>318922</xdr:colOff>
+      <xdr:colOff>242722</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>91636</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="709810" cy="235193"/>
+    <xdr:ext cx="883383" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="93" name="CuadroTexto 92">
@@ -2114,8 +2131,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9462922" y="91636"/>
-          <a:ext cx="709810" cy="235193"/>
+          <a:off x="9386722" y="91636"/>
+          <a:ext cx="883383" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2144,12 +2161,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Dashboard</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2159,11 +2178,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>557047</xdr:colOff>
+      <xdr:colOff>376072</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>91636</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1146981" cy="235193"/>
+    <xdr:ext cx="1531638" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="94" name="CuadroTexto 93">
@@ -2177,8 +2196,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8939047" y="853636"/>
-          <a:ext cx="1146981" cy="235193"/>
+          <a:off x="8758072" y="853636"/>
+          <a:ext cx="1531638" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2207,12 +2226,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Admon. Proveedores</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2222,11 +2243,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="850426" cy="235193"/>
+    <xdr:ext cx="1100686" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="95" name="CuadroTexto 94">
@@ -2240,8 +2261,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9305925" y="1552575"/>
-          <a:ext cx="850426" cy="235193"/>
+          <a:off x="9191625" y="1552575"/>
+          <a:ext cx="1100686" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2270,12 +2291,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Notificaciones</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2285,11 +2308,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="831894" cy="235193"/>
+    <xdr:ext cx="1069075" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="96" name="CuadroTexto 95">
@@ -2303,8 +2326,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11106150" y="85725"/>
-          <a:ext cx="831894" cy="235193"/>
+          <a:off x="10972800" y="85725"/>
+          <a:ext cx="1069075" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2333,12 +2356,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Multilenguaje</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2352,7 +2377,7 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="918521" cy="235193"/>
+    <xdr:ext cx="1184042" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="97" name="CuadroTexto 96">
@@ -2367,7 +2392,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11372850" y="771525"/>
-          <a:ext cx="918521" cy="235193"/>
+          <a:ext cx="1184042" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2396,12 +2421,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Roles y Perfiles</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2411,11 +2438,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:colOff>619125</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="984950" cy="235193"/>
+    <xdr:ext cx="1299074" cy="232628"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="98" name="CuadroTexto 97">
@@ -2429,8 +2456,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11315700" y="1504950"/>
-          <a:ext cx="984950" cy="235193"/>
+          <a:off x="11287125" y="1504950"/>
+          <a:ext cx="1299074" cy="232628"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2459,12 +2486,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-CO" sz="900" b="1" baseline="0">
-              <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Expansión Global</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="900" b="1">
-            <a:latin typeface="Ink Free" panose="03080402000500000000" pitchFamily="66" charset="0"/>
+            <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
       </xdr:txBody>
@@ -2814,7 +2843,7 @@
   <dimension ref="T34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>